<commit_message>
Syncing a bunch of old files
I think these are all old files.
</commit_message>
<xml_diff>
--- a/all_rxns_v5.xlsx
+++ b/all_rxns_v5.xlsx
@@ -1,15 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Lynd Lab research\Ctherm CBP project\thermodynamic analysis with Satya 11-30-2018\Ctherm_thermo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB072050-1121-40FB-9DB7-B57776589624}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -469,8 +483,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,6 +547,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -579,7 +601,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -611,9 +633,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,6 +685,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -820,14 +878,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32:H36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="103.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="64.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,7 +917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -873,7 +940,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -893,7 +960,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -913,7 +980,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -933,7 +1000,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -953,7 +1020,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -973,7 +1040,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -993,7 +1060,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1013,7 +1080,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1033,7 +1100,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1053,7 +1120,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1076,7 +1143,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1096,7 +1163,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1116,7 +1183,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1136,7 +1203,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1156,7 +1223,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1176,7 +1243,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1196,7 +1263,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1216,7 +1283,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1236,7 +1303,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1256,7 +1323,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1276,7 +1343,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1296,7 +1363,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1316,7 +1383,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1336,7 +1403,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1356,7 +1423,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1376,7 +1443,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1396,7 +1463,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1416,7 +1483,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1436,7 +1503,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1459,7 +1526,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1476,7 +1543,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1493,7 +1560,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1510,7 +1577,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1527,7 +1594,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>

</xml_diff>